<commit_message>
Update daily work details
</commit_message>
<xml_diff>
--- a/doc/wt/Details.xlsx
+++ b/doc/wt/Details.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Double\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1025\github\temcocontrols\T3000Webview\doc\wt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF0CF97-E9E1-4E59-BD72-1D57D0B11931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31510DB3-0A24-4743-A78F-4B9DBACCEF4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="147">
   <si>
     <t>周</t>
   </si>
@@ -395,6 +395,81 @@
   </si>
   <si>
     <t>2. Fixed typo and updated the work details.</t>
+  </si>
+  <si>
+    <t>1. Added more events to the device and graphic panel, simulated how to load real data, send message and process the data.</t>
+  </si>
+  <si>
+    <t>1. Added new functions to load the dynamic element count for each graphic panel.</t>
+  </si>
+  <si>
+    <t>2. Updated the communication type of socket client for sending real message to T3000.</t>
+  </si>
+  <si>
+    <t>2025-01-06/07</t>
+  </si>
+  <si>
+    <t>2. Added new functions to load the dynamic element count for each graphic panel.</t>
+  </si>
+  <si>
+    <t>3. Updated the communication type of socket client for sending real message to T3000.</t>
+  </si>
+  <si>
+    <t>1. Updated socket server with following functions:</t>
+  </si>
+  <si>
+    <t># Add data model MessageModel to handle the message content &amp; Add relate events to send the message to T3000</t>
+  </si>
+  <si>
+    <t># Update rust socket server and add bind client function to store the client info</t>
+  </si>
+  <si>
+    <t># Update process message function to bind the client info</t>
+  </si>
+  <si>
+    <t>1. Updated socket server and webview with following changes:</t>
+  </si>
+  <si>
+    <t># Keep the orgin ui layout when open the webview from T3000</t>
+  </si>
+  <si>
+    <t># Update socket message type set BIND_DEVICE=13</t>
+  </si>
+  <si>
+    <t># Update rust server to block wrong format messages</t>
+  </si>
+  <si>
+    <t># Update device panel with real device data</t>
+  </si>
+  <si>
+    <t>1. Tried to fix error: Message payload is larger than the default config size =&gt;</t>
+  </si>
+  <si>
+    <t>Currently this results in an error like Capacity(MessageTooLong { size: 2319073409, max_size: 16777216 }) on the receiving end</t>
+  </si>
+  <si>
+    <t>Struct tungstenite::protocol::WebSocketConfig</t>
+  </si>
+  <si>
+    <t>https://docs.rs/tungstenite/0.21.0/tungstenite/protocol/struct.WebSocketConfig.html</t>
+  </si>
+  <si>
+    <t>2. Result returned in a incorrect format, should including action field and the error field with text content also.</t>
+  </si>
+  <si>
+    <t>3. Need to set the device connection type to wifi to get the panel list info. this is not working under USB model.</t>
+  </si>
+  <si>
+    <t>1. Updated the socket server and bind real device info to webview</t>
+  </si>
+  <si>
+    <t>2. Added functions monitor_clients_status &amp; check_clients_status for monitoring the server status</t>
+  </si>
+  <si>
+    <t>1. Updated graphic ui</t>
+  </si>
+  <si>
+    <t>2. Updated save logic for both external browser and built in browser</t>
   </si>
 </sst>
 </file>
@@ -462,7 +537,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -474,15 +549,16 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -763,15 +839,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" customWidth="1"/>
+    <col min="1" max="1" width="6.109375" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" customWidth="1"/>
     <col min="3" max="3" width="11.77734375" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
@@ -955,101 +1031,107 @@
       <c r="A13" s="2">
         <v>10</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>45649</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>45653</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="2">
         <v>5</v>
       </c>
-      <c r="E13" s="7"/>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2">
         <v>11</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <v>45656</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>45657</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="6">
         <v>2</v>
       </c>
-      <c r="E14" s="7"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2">
         <v>12</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B16" s="5">
         <v>45659</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="5">
         <v>45660</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="6">
         <v>2</v>
       </c>
-      <c r="E16" s="7"/>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2">
+        <v>13</v>
+      </c>
+      <c r="B17" s="5">
+        <v>45663</v>
+      </c>
+      <c r="C17" s="5">
+        <v>45667</v>
+      </c>
+      <c r="D17" s="7">
+        <v>5</v>
+      </c>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:5">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:5">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:5">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:5">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:5">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:5">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:5">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:5">
       <c r="A26" s="1"/>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:5">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:5">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:5">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:5">
       <c r="A30" s="1"/>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" s="1"/>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1959,13 +2041,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B367D133-EDA4-4AEB-BA43-774273F016B7}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="10.109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1">
@@ -2012,6 +2097,171 @@
         <v>121</v>
       </c>
     </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="1">
+        <v>45663</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="1">
+        <v>45664</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="1">
+        <v>45665</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="1">
+        <v>45666</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="1">
+        <v>45667</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="1">
+        <v>45670</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="1">
+        <v>45671</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>146</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update daily work summary of 25.01.13-01.19
</commit_message>
<xml_diff>
--- a/doc/wt/Details.xlsx
+++ b/doc/wt/Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1025\github\temcocontrols\T3000Webview\doc\wt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31510DB3-0A24-4743-A78F-4B9DBACCEF4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C20143-7AD2-4D84-A878-2512CE5D0628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="171">
   <si>
     <t>周</t>
   </si>
@@ -470,6 +470,78 @@
   </si>
   <si>
     <t>2. Updated save logic for both external browser and built in browser</t>
+  </si>
+  <si>
+    <t>1. Updated GET_ENTITY message type</t>
+  </si>
+  <si>
+    <t>2. Updated socket client and send GET_ENTITIES to T3</t>
+  </si>
+  <si>
+    <t>3. Updated daily work details</t>
+  </si>
+  <si>
+    <t>4. Added serial_number and set the graphic index start with 1</t>
+  </si>
+  <si>
+    <t>1. Updated index page and migrate code</t>
+  </si>
+  <si>
+    <t>2. Fixed bugs</t>
+  </si>
+  <si>
+    <t>3. Added new function ProcessWebSocketFrame</t>
+  </si>
+  <si>
+    <t>4. Added clearGetPanelsInterval</t>
+  </si>
+  <si>
+    <t>1. Refactored code of webview2 and split them into different files</t>
+  </si>
+  <si>
+    <t>2. Added webview2 message handler</t>
+  </si>
+  <si>
+    <t>3. Added functions to handle webview2 incoming message</t>
+  </si>
+  <si>
+    <t>1. Updated test page's libs references</t>
+  </si>
+  <si>
+    <t>2. Added property $q to store the quasar framework instance</t>
+  </si>
+  <si>
+    <t>3. Updated functions for counting graphic element count</t>
+  </si>
+  <si>
+    <t>1. Updated WebSocketClient and WebViewClient</t>
+  </si>
+  <si>
+    <t>2. Updated websocketclient-SaveLibraryData</t>
+  </si>
+  <si>
+    <t>3. Updated T3UpdateEntryField, reloadPanelsData, newProject</t>
+  </si>
+  <si>
+    <t>1. Updated device panel and add error section</t>
+  </si>
+  <si>
+    <t>2. Updated save function to automatically save every 30s</t>
+  </si>
+  <si>
+    <t>3. Updated the graphic selection logic, add presets function to avoid load incorrect initial data</t>
+  </si>
+  <si>
+    <t>1. Merged and optimized code for version release.</t>
+  </si>
+  <si>
+    <t>2. Fixed bug [Put the ‘Linked with’ section up top]. (already done)</t>
+  </si>
+  <si>
+    <t>3. Tried to fix bug [Did not remember the last position and size]. (50%)</t>
+  </si>
+  <si>
+    <t>4. About the wall part, I want to fix it along with the new UI. The libs has some parts that need to be updated, this part may not be done before the holiday.</t>
   </si>
 </sst>
 </file>
@@ -555,10 +627,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -842,12 +914,12 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="6.109375" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" customWidth="1"/>
     <col min="3" max="3" width="11.77734375" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
@@ -1089,16 +1161,34 @@
       <c r="C17" s="5">
         <v>45667</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="6">
         <v>5</v>
       </c>
-      <c r="E17" s="8"/>
+      <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="1"/>
+      <c r="A18" s="2">
+        <v>14</v>
+      </c>
+      <c r="B18" s="5">
+        <v>45670</v>
+      </c>
+      <c r="C18" s="5">
+        <v>45676</v>
+      </c>
+      <c r="D18" s="8">
+        <v>6</v>
+      </c>
+      <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="1"/>
+      <c r="A19" s="2">
+        <v>15</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1"/>
@@ -2041,10 +2131,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B367D133-EDA4-4AEB-BA43-774273F016B7}">
-  <dimension ref="A1:A53"/>
+  <dimension ref="A1:A91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55:A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2262,6 +2352,161 @@
         <v>146</v>
       </c>
     </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="1">
+        <v>45672</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="1">
+        <v>45673</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="1">
+        <v>45674</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="1">
+        <v>45675</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" s="1">
+        <v>45676</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="1">
+        <v>45677</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" s="1">
+        <v>45678</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" t="s">
+        <v>170</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>